<commit_message>
Partial execution and adjustments
</commit_message>
<xml_diff>
--- a/AutomationFramework/results/21102020/excel_logs/network_instance_test_ni_bgp_test_ni_bgp_as_logs.xlsx
+++ b/AutomationFramework/results/21102020/excel_logs/network_instance_test_ni_bgp_test_ni_bgp_as_logs.xlsx
@@ -510,7 +510,7 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t xml:space="preserve">&lt;rpc-reply message-id="urn:uuid:9f1c07fb-e75e-48a3-ae1a-b70201251b4d"&gt;
+          <t xml:space="preserve">&lt;rpc-reply message-id="urn:uuid:0b4d6dd8-568f-4368-8f65-7b6d15809b2b"&gt;
   &lt;data/&gt;
 &lt;/rpc-reply&gt;
 </t>
@@ -532,11 +532,11 @@
           &lt;/config&gt;
           &lt;protocols&gt;
             &lt;protocol&gt;
-              &lt;identifier&gt;BGP&lt;/identifier&gt;
-              &lt;name&gt;BGP_65000&lt;/name&gt;
+              &lt;identifier xmlns:oc-pol-types="http://openconfig.net/yang/policy-types"&gt;oc-pol-types:BGP&lt;/identifier&gt;
+              &lt;name&gt;default&lt;/name&gt;
               &lt;config&gt;
                 &lt;identifier xmlns:oc-pol-types="http://openconfig.net/yang/policy-types"&gt;oc-pol-types:BGP&lt;/identifier&gt;
-                &lt;name&gt;BGP_65000&lt;/name&gt;
+                &lt;name&gt;default&lt;/name&gt;
               &lt;/config&gt;
               &lt;bgp&gt;
                 &lt;global&gt;

</xml_diff>